<commit_message>
Corrección en el backlog
</commit_message>
<xml_diff>
--- a/Documentación/PREGAME/1. ELICITACION/1.6 Backlog/7185_G2_Basantes_Orellana_Lopez_Backlog-Sprint1_v3.0.xlsx
+++ b/Documentación/PREGAME/1. ELICITACION/1.6 Backlog/7185_G2_Basantes_Orellana_Lopez_Backlog-Sprint1_v3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ANALISIS Y DISEÑO\7185_G2\Documentación\PREGAME\1. ELICITACION\1.6 Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC7D513C-26E9-46C0-A4B9-AE5D66CAFA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8D2D9C-D4FF-4D27-8D3B-DB709C02FAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -513,8 +513,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1099,7 +1099,9 @@
   </sheetPr>
   <dimension ref="A1:H994"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2389,12 +2391,14 @@
   </sheetPr>
   <dimension ref="A1:I916"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C34" sqref="C34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="61" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="64.140625" customWidth="1"/>
   </cols>
@@ -2495,7 +2499,7 @@
       <c r="B7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="21"/>
@@ -2621,7 +2625,7 @@
       <c r="B14" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D14" s="21"/>
@@ -2655,7 +2659,7 @@
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
@@ -2751,7 +2755,7 @@
       <c r="B21" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D21" s="21"/>
@@ -2845,7 +2849,7 @@
     </row>
     <row r="29" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="4"/>
-      <c r="C29" s="22"/>
+      <c r="C29" s="23"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
@@ -2925,7 +2929,7 @@
     </row>
     <row r="37" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="4"/>
-      <c r="C37" s="23"/>
+      <c r="C37" s="22"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
@@ -3863,6 +3867,16 @@
     <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
     <mergeCell ref="C36:F36"/>
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C41:F41"/>
@@ -3875,16 +3889,6 @@
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="C34:F34"/>
     <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -3895,7 +3899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1223DE8A-43F8-4644-BFC6-EAA17368D118}">
   <dimension ref="A2:J43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -4040,7 +4044,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="22"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
@@ -4194,7 +4198,7 @@
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="23"/>
+      <c r="C16" s="22"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
@@ -4421,6 +4425,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
     <mergeCell ref="C21:F21"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C13:F13"/>
@@ -4428,8 +4434,6 @@
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4442,8 +4446,8 @@
   </sheetPr>
   <dimension ref="B1:I988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>